<commit_message>
nktc hanh chính công
</commit_message>
<xml_diff>
--- a/nktc.xlsx
+++ b/nktc.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\QuanProject\qlcl project git\qlcl_project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF4B84F-4644-46A6-8F8A-00E9C6D48BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="690" yWindow="4215" windowWidth="20535" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1066,11 +1085,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1134,6 +1153,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1180,7 +1207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1212,9 +1239,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1246,6 +1291,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1421,14 +1484,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G208"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44470</v>
       </c>
@@ -1462,7 +1530,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44471</v>
       </c>
@@ -1476,7 +1544,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44472</v>
       </c>
@@ -1490,7 +1558,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44473</v>
       </c>
@@ -1504,7 +1572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44474</v>
       </c>
@@ -1518,7 +1586,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44475</v>
       </c>
@@ -1535,7 +1603,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44476</v>
       </c>
@@ -1549,7 +1617,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44477</v>
       </c>
@@ -1569,7 +1637,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44478</v>
       </c>
@@ -1589,7 +1657,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44479</v>
       </c>
@@ -1606,7 +1674,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44480</v>
       </c>
@@ -1623,7 +1691,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44481</v>
       </c>
@@ -1643,7 +1711,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44482</v>
       </c>
@@ -1660,7 +1728,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44483</v>
       </c>
@@ -1677,7 +1745,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44484</v>
       </c>
@@ -1697,7 +1765,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44485</v>
       </c>
@@ -1717,7 +1785,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44486</v>
       </c>
@@ -1734,7 +1802,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44487</v>
       </c>
@@ -1751,7 +1819,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44488</v>
       </c>
@@ -1771,7 +1839,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44489</v>
       </c>
@@ -1782,7 +1850,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44490</v>
       </c>
@@ -1793,7 +1861,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44491</v>
       </c>
@@ -1804,7 +1872,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44492</v>
       </c>
@@ -1815,7 +1883,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44493</v>
       </c>
@@ -1826,7 +1894,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44494</v>
       </c>
@@ -1837,7 +1905,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44495</v>
       </c>
@@ -1848,7 +1916,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44496</v>
       </c>
@@ -1859,7 +1927,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44497</v>
       </c>
@@ -1870,7 +1938,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44498</v>
       </c>
@@ -1881,7 +1949,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44499</v>
       </c>
@@ -1892,7 +1960,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44500</v>
       </c>
@@ -1903,7 +1971,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44501</v>
       </c>
@@ -1917,7 +1985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44502</v>
       </c>
@@ -1931,7 +1999,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44503</v>
       </c>
@@ -1945,7 +2013,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44504</v>
       </c>
@@ -1962,7 +2030,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44505</v>
       </c>
@@ -1976,7 +2044,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44506</v>
       </c>
@@ -1990,7 +2058,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44507</v>
       </c>
@@ -2004,7 +2072,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44508</v>
       </c>
@@ -2018,7 +2086,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44509</v>
       </c>
@@ -2032,7 +2100,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44510</v>
       </c>
@@ -2046,7 +2114,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44511</v>
       </c>
@@ -2060,7 +2128,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44512</v>
       </c>
@@ -2074,7 +2142,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44513</v>
       </c>
@@ -2088,7 +2156,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44514</v>
       </c>
@@ -2102,7 +2170,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44515</v>
       </c>
@@ -2116,7 +2184,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44516</v>
       </c>
@@ -2130,7 +2198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44517</v>
       </c>
@@ -2150,7 +2218,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44518</v>
       </c>
@@ -2167,7 +2235,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44519</v>
       </c>
@@ -2181,7 +2249,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44520</v>
       </c>
@@ -2198,7 +2266,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44521</v>
       </c>
@@ -2218,7 +2286,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44522</v>
       </c>
@@ -2232,7 +2300,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44523</v>
       </c>
@@ -2246,7 +2314,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44524</v>
       </c>
@@ -2263,7 +2331,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44525</v>
       </c>
@@ -2283,7 +2351,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44526</v>
       </c>
@@ -2297,7 +2365,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44527</v>
       </c>
@@ -2317,7 +2385,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44528</v>
       </c>
@@ -2337,7 +2405,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44529</v>
       </c>
@@ -2354,7 +2422,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44530</v>
       </c>
@@ -2371,7 +2439,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44531</v>
       </c>
@@ -2391,7 +2459,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44532</v>
       </c>
@@ -2411,7 +2479,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44533</v>
       </c>
@@ -2428,7 +2496,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44534</v>
       </c>
@@ -2448,7 +2516,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44535</v>
       </c>
@@ -2468,7 +2536,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44536</v>
       </c>
@@ -2488,7 +2556,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44537</v>
       </c>
@@ -2502,7 +2570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44538</v>
       </c>
@@ -2516,7 +2584,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44539</v>
       </c>
@@ -2536,7 +2604,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44540</v>
       </c>
@@ -2556,7 +2624,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44541</v>
       </c>
@@ -2576,7 +2644,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>44542</v>
       </c>
@@ -2590,7 +2658,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44543</v>
       </c>
@@ -2604,7 +2672,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44544</v>
       </c>
@@ -2618,7 +2686,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>44545</v>
       </c>
@@ -2638,7 +2706,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44546</v>
       </c>
@@ -2658,7 +2726,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>44547</v>
       </c>
@@ -2672,7 +2740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>44548</v>
       </c>
@@ -2692,7 +2760,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44549</v>
       </c>
@@ -2712,7 +2780,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44550</v>
       </c>
@@ -2732,7 +2800,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>44551</v>
       </c>
@@ -2746,7 +2814,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44552</v>
       </c>
@@ -2763,7 +2831,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44553</v>
       </c>
@@ -2783,7 +2851,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>44554</v>
       </c>
@@ -2800,7 +2868,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44555</v>
       </c>
@@ -2814,7 +2882,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>44556</v>
       </c>
@@ -2828,7 +2896,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>44557</v>
       </c>
@@ -2845,7 +2913,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44558</v>
       </c>
@@ -2865,7 +2933,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44559</v>
       </c>
@@ -2885,7 +2953,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>44560</v>
       </c>
@@ -2905,7 +2973,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>44561</v>
       </c>
@@ -2916,7 +2984,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44562</v>
       </c>
@@ -2927,7 +2995,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>44563</v>
       </c>
@@ -2944,7 +3012,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>44564</v>
       </c>
@@ -2964,7 +3032,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>44565</v>
       </c>
@@ -2981,7 +3049,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>44566</v>
       </c>
@@ -3001,7 +3069,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>44567</v>
       </c>
@@ -3015,7 +3083,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>44568</v>
       </c>
@@ -3035,7 +3103,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>44569</v>
       </c>
@@ -3052,7 +3120,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>44570</v>
       </c>
@@ -3069,7 +3137,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>44571</v>
       </c>
@@ -3083,7 +3151,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>44572</v>
       </c>
@@ -3097,7 +3165,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>44573</v>
       </c>
@@ -3114,7 +3182,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>44574</v>
       </c>
@@ -3134,7 +3202,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>44575</v>
       </c>
@@ -3148,7 +3216,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>44576</v>
       </c>
@@ -3162,7 +3230,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>44577</v>
       </c>
@@ -3176,7 +3244,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>44578</v>
       </c>
@@ -3190,7 +3258,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>44579</v>
       </c>
@@ -3207,7 +3275,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>44580</v>
       </c>
@@ -3227,7 +3295,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>44581</v>
       </c>
@@ -3238,7 +3306,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>44582</v>
       </c>
@@ -3252,7 +3320,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>44583</v>
       </c>
@@ -3266,7 +3334,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>44584</v>
       </c>
@@ -3280,7 +3348,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>44585</v>
       </c>
@@ -3291,7 +3359,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>44586</v>
       </c>
@@ -3308,7 +3376,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>44587</v>
       </c>
@@ -3328,7 +3396,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>44588</v>
       </c>
@@ -3342,7 +3410,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>44589</v>
       </c>
@@ -3359,7 +3427,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>44590</v>
       </c>
@@ -3379,7 +3447,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>44591</v>
       </c>
@@ -3393,7 +3461,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>44592</v>
       </c>
@@ -3407,7 +3475,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>44593</v>
       </c>
@@ -3418,7 +3486,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>44594</v>
       </c>
@@ -3429,7 +3497,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>44595</v>
       </c>
@@ -3440,7 +3508,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>44596</v>
       </c>
@@ -3451,7 +3519,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>44597</v>
       </c>
@@ -3462,7 +3530,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>44598</v>
       </c>
@@ -3473,7 +3541,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>44599</v>
       </c>
@@ -3490,7 +3558,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>44600</v>
       </c>
@@ -3504,7 +3572,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>44601</v>
       </c>
@@ -3518,7 +3586,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>44602</v>
       </c>
@@ -3532,7 +3600,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>44603</v>
       </c>
@@ -3546,7 +3614,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>44604</v>
       </c>
@@ -3560,7 +3628,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>44605</v>
       </c>
@@ -3574,7 +3642,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>44606</v>
       </c>
@@ -3588,7 +3656,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>44607</v>
       </c>
@@ -3602,7 +3670,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>44608</v>
       </c>
@@ -3619,7 +3687,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>44609</v>
       </c>
@@ -3633,7 +3701,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>44610</v>
       </c>
@@ -3650,7 +3718,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>44611</v>
       </c>
@@ -3667,7 +3735,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>44612</v>
       </c>
@@ -3684,7 +3752,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>44613</v>
       </c>
@@ -3698,7 +3766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>44614</v>
       </c>
@@ -3712,7 +3780,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>44615</v>
       </c>
@@ -3726,7 +3794,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>44616</v>
       </c>
@@ -3740,7 +3808,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>44617</v>
       </c>
@@ -3757,7 +3825,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>44618</v>
       </c>
@@ -3774,7 +3842,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>44619</v>
       </c>
@@ -3788,7 +3856,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>44620</v>
       </c>
@@ -3802,7 +3870,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>44621</v>
       </c>
@@ -3819,7 +3887,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>44622</v>
       </c>
@@ -3833,7 +3901,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>44623</v>
       </c>
@@ -3853,7 +3921,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>44624</v>
       </c>
@@ -3870,7 +3938,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>44625</v>
       </c>
@@ -3884,7 +3952,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>44626</v>
       </c>
@@ -3901,7 +3969,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>44627</v>
       </c>
@@ -3915,7 +3983,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>44628</v>
       </c>
@@ -3932,7 +4000,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>44629</v>
       </c>
@@ -3949,7 +4017,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>44630</v>
       </c>
@@ -3963,7 +4031,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>44631</v>
       </c>
@@ -3980,7 +4048,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>44632</v>
       </c>
@@ -3994,7 +4062,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>44633</v>
       </c>
@@ -4014,7 +4082,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>44634</v>
       </c>
@@ -4034,7 +4102,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>44635</v>
       </c>
@@ -4051,7 +4119,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>44636</v>
       </c>
@@ -4065,7 +4133,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>44637</v>
       </c>
@@ -4079,7 +4147,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>44638</v>
       </c>
@@ -4096,7 +4164,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>44639</v>
       </c>
@@ -4113,7 +4181,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>44640</v>
       </c>
@@ -4127,7 +4195,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>44641</v>
       </c>
@@ -4141,7 +4209,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>44642</v>
       </c>
@@ -4158,7 +4226,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>44643</v>
       </c>
@@ -4172,7 +4240,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>44644</v>
       </c>
@@ -4186,7 +4254,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>44645</v>
       </c>
@@ -4206,7 +4274,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>44646</v>
       </c>
@@ -4223,7 +4291,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>44647</v>
       </c>
@@ -4240,7 +4308,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>44648</v>
       </c>
@@ -4254,7 +4322,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>44649</v>
       </c>
@@ -4268,7 +4336,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>44650</v>
       </c>
@@ -4282,7 +4350,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>44651</v>
       </c>
@@ -4299,7 +4367,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>44652</v>
       </c>
@@ -4319,7 +4387,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>44653</v>
       </c>
@@ -4336,7 +4404,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>44654</v>
       </c>
@@ -4353,7 +4421,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>44655</v>
       </c>
@@ -4373,7 +4441,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>44656</v>
       </c>
@@ -4390,7 +4458,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>44657</v>
       </c>
@@ -4407,7 +4475,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>44658</v>
       </c>
@@ -4424,7 +4492,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>44659</v>
       </c>
@@ -4441,7 +4509,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>44660</v>
       </c>
@@ -4455,7 +4523,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>44661</v>
       </c>
@@ -4475,7 +4543,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>44662</v>
       </c>
@@ -4492,7 +4560,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>44663</v>
       </c>
@@ -4509,7 +4577,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>44664</v>
       </c>
@@ -4526,7 +4594,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>44665</v>
       </c>
@@ -4546,7 +4614,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>44666</v>
       </c>
@@ -4566,7 +4634,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>44667</v>
       </c>
@@ -4583,7 +4651,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>44668</v>
       </c>
@@ -4600,7 +4668,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>44669</v>
       </c>
@@ -4620,7 +4688,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>44670</v>
       </c>
@@ -4637,7 +4705,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>44671</v>
       </c>
@@ -4657,7 +4725,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>44672</v>
       </c>
@@ -4674,7 +4742,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>44673</v>
       </c>
@@ -4688,7 +4756,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>44674</v>
       </c>
@@ -4705,7 +4773,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>44675</v>
       </c>
@@ -4722,7 +4790,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>44676</v>
       </c>
@@ -4733,6 +4801,97 @@
         <v>210</v>
       </c>
     </row>
+    <row r="209" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="224" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="226" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="227" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="228" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="229" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="230" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="231" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="232" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="233" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="234" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="235" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="236" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="237" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="238" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="239" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="240" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="241" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="242" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="243" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="244" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="245" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="246" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="247" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="248" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="249" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="250" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="251" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="252" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="253" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="254" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="255" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="256" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="257" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="258" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="259" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="260" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="261" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="262" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="263" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="264" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="265" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="266" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="267" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="268" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="269" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="270" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="271" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="272" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="273" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="274" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="275" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="276" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="277" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="278" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="279" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="280" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="281" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="282" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="283" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="285" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="286" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="287" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="288" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="289" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="290" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="291" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="292" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="293" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="294" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="295" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="296" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="297" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="298" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="299" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>